<commit_message>
create register event crud
</commit_message>
<xml_diff>
--- a/src/upload/dataEvents.xlsx
+++ b/src/upload/dataEvents.xlsx
@@ -11,15 +11,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>prueba 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+  <si>
+    <t>id_event</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>id_city</t>
+  </si>
+  <si>
+    <t>Prueba edited1</t>
+  </si>
+  <si>
+    <t>Prueba load 1 description</t>
+  </si>
+  <si>
+    <t>2024-11-12</t>
+  </si>
+  <si>
+    <t>3:00 pm</t>
+  </si>
+  <si>
+    <t>Calle 1</t>
+  </si>
+  <si>
+    <t>Prueba edited 2</t>
+  </si>
+  <si>
+    <t>Prueba load 2 descriptio</t>
+  </si>
+  <si>
+    <t>2024-10-13</t>
+  </si>
+  <si>
+    <t>Calle 2</t>
+  </si>
+  <si>
+    <t>Prueba edited 3</t>
+  </si>
+  <si>
+    <t>Prueba load 3 description</t>
+  </si>
+  <si>
+    <t>2024-12-14</t>
+  </si>
+  <si>
+    <t>Calle 3</t>
   </si>
 </sst>
 </file>
@@ -53,11 +104,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -275,6 +329,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="22.5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -283,13 +340,87 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1">
         <v>1.0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>